<commit_message>
Update WebGui_FwUpDnGradeFunctionTest.cs  - Add sleep 10 second when test is completed
</commit_message>
<xml_diff>
--- a/CyberRouterATE/bin/Debug/testCondition/FwStress/FwStressSteps.xlsx
+++ b/CyberRouterATE/bin/Debug/testCondition/FwStress/FwStressSteps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10248" yWindow="672" windowWidth="10272" windowHeight="7332"/>
+    <workbookView xWindow="10248" yWindow="732" windowWidth="10272" windowHeight="7272"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -547,7 +547,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>

</xml_diff>